<commit_message>
Update: replace data files and scripts; remove subfamily.xlsx
</commit_message>
<xml_diff>
--- a/authors_per_year.xlsx
+++ b/authors_per_year.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaobiosmac/Desktop/R/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaobiosmac/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F9DEE7-EAAD-2849-813D-886620752219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89EA3858-2C9C-7346-B86A-DAA98D7A51DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="24400" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -451,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -814,6 +814,20 @@
         <v>13</v>
       </c>
     </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>2024</v>
+      </c>
+      <c r="B26" s="4">
+        <v>7</v>
+      </c>
+      <c r="C26" s="4">
+        <v>39</v>
+      </c>
+      <c r="D26" s="4">
+        <v>7.14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>